<commit_message>
Adding places with coordinates into Excel Sheet
</commit_message>
<xml_diff>
--- a/FoliumMaps/Coordinates.xlsx
+++ b/FoliumMaps/Coordinates.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dasaw\Documents\Python\Untitled Folder\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dasaw\Documents\Python\FoliumMaps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6AB6E5E-4C35-457B-B5E1-AE17D2C4CE31}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73CFCE3-BA46-474B-BF22-861D3DCF55A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="15375" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t xml:space="preserve">PlaceName </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Longitude</t>
   </si>
@@ -36,7 +33,22 @@
     <t>Latitude</t>
   </si>
   <si>
-    <t>MGF mall, Gurgaon</t>
+    <t>PlaceName</t>
+  </si>
+  <si>
+    <t>City Center Shopping Mall</t>
+  </si>
+  <si>
+    <t>MGF Metropolitan Mall</t>
+  </si>
+  <si>
+    <t>DT City Center Mall</t>
+  </si>
+  <si>
+    <t>MGF Mega Mall</t>
+  </si>
+  <si>
+    <t>Sahara Mall</t>
   </si>
 </sst>
 </file>
@@ -363,10 +375,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,24 +390,68 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>28.480908500000002</v>
       </c>
       <c r="C2">
         <v>77.078091099999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>28.487140799999999</v>
+      </c>
+      <c r="C3">
+        <v>77.090245600000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>28.4789745</v>
+      </c>
+      <c r="C4">
+        <v>77.078437500000007</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>28.479719599999999</v>
+      </c>
+      <c r="C5">
+        <v>77.0871736</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>28.479558699999998</v>
+      </c>
+      <c r="C6">
+        <v>77.084565799999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>